<commit_message>
Add phone number formatting and validation logic.
</commit_message>
<xml_diff>
--- a/resultant_excel.xlsx
+++ b/resultant_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,31 +507,31 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
+          <t>Charlie Brown</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>9660177109</t>
+          <t>8107331777</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>alice.johnson@example.com</t>
+          <t>vinayak_sharma@technologymindz.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Alice is interested in the premium package that includes advanced analytics, priority support, and additional storage capacity. She wants a detailed demo before making the decision.</t>
+          <t>Charlie is evaluating enterprise-level solutions with a strong emphasis on scalability, integration with his existing ERP system, and compliance with international data protection regulations. He also needs a custom training program for his team.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -539,113 +539,37 @@
           <t>no-answer</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>91</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Healthcare</t>
+          <t>Real Estate</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>ABC Company</t>
+          <t>XYZ Company Ltd.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Texas, USA</t>
+          <t>Berlin, Germany</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
+          <t>Charlie has shown strong interest in a long-term partnership if the enterprise solution aligns with his company’s compliance and integration needs. He mentioned that decision-making will involve multiple stakeholders, and the procurement cycle might take up to three months. We should prepare detailed documentation, case studies, and a tailored presentation for his board of directors.
+[2025-08-25 17:13:21] No summary available. Conversation transcript missing.</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
           <t>nan
-[2025-08-23 17:01:26] No summary available. Conversation transcript missing.</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-[2025-08-23 17:01:26] No tasks found for this call.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>37</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Charlie Brown</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>8107331777</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>charlie.brown@example.com</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Charlie is evaluating enterprise-level solutions with a strong emphasis on scalability, integration with his existing ERP system, and compliance with international data protection regulations. He also needs a custom training program for his team.</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>busy</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>91</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Real Estate</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>XYZ Company Ltd.</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Berlin, Germany</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Charlie has shown strong interest in a long-term partnership if the enterprise solution aligns with his company’s compliance and integration needs. He mentioned that decision-making will involve multiple stakeholders, and the procurement cycle might take up to three months. We should prepare detailed documentation, case studies, and a tailored presentation for his board of directors.
-[2025-08-23 17:01:45] No summary available. Conversation transcript missing.</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-[2025-08-23 17:01:45] No tasks found for this call.</t>
+[2025-08-25 17:13:21] No tasks found for this call.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor conversation transcript summarization logic and enhance task extraction process
</commit_message>
<xml_diff>
--- a/resultant_excel.xlsx
+++ b/resultant_excel.xlsx
@@ -507,16 +507,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Charlie Brown</t>
+          <t>Bhavesh</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -531,28 +531,32 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Charlie is evaluating enterprise-level solutions with a strong emphasis on scalability, integration with his existing ERP system, and compliance with international data protection regulations. He also needs a custom training program for his team.</t>
+          <t>bhavesh is interested in the premium package that includes advanced analytics, priority support, and additional storage capacity. She wants a detailed demo before making the decision.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>no-answer</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Real Estate</t>
+          <t>Healthcare</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>XYZ Company Ltd.</t>
+          <t>ABC Company</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Berlin, Germany</t>
+          <t>Texas, USA</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -562,14 +566,14 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Charlie has shown strong interest in a long-term partnership if the enterprise solution aligns with his company’s compliance and integration needs. He mentioned that decision-making will involve multiple stakeholders, and the procurement cycle might take up to three months. We should prepare detailed documentation, case studies, and a tailored presentation for his board of directors.
-[2025-08-25 17:13:21] No summary available. Conversation transcript missing.</t>
+          <t>nan
+[2025-08-25 22:45:02] The customer is interested in the premium package and wants to schedule a meeting with a representative. The meeting is scheduled for the next day at 4 p.m.</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
           <t>nan
-[2025-08-25 17:13:21] No tasks found for this call.</t>
+[2025-08-25 22:45:02] 1. Schedule a meeting with a representative, 2. Send a meeting invitation to the customer's email</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added mid call excel download
</commit_message>
<xml_diff>
--- a/resultant_excel.xlsx
+++ b/resultant_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,7 +507,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bhavesh</t>
+          <t>vinayak</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -531,7 +531,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>bhavesh is interested in the premium package that includes advanced analytics, priority support, and additional storage capacity. She wants a detailed demo before making the decision.</t>
+          <t>Alice is interested in the premium package that includes advanced analytics, priority support, and additional storage capacity. She wants a detailed demo before making the decision.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -566,14 +566,78 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>nan
-[2025-08-25 22:45:02] The customer is interested in the premium package and wants to schedule a meeting with a representative. The meeting is scheduled for the next day at 4 p.m.</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>nan
-[2025-08-25 22:45:02] 1. Schedule a meeting with a representative, 2. Send a meeting invitation to the customer's email</t>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>vipul</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>9977183691</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>vinayak_sharma@technologymindz.com</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Charlie is evaluating enterprise-level solutions with a strong emphasis on scalability, integration with his existing ERP system, and compliance with international data protection regulations. He also needs a custom training program for his team.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Real Estate</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>XYZ Company Ltd.</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Berlin, Germany</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Charlie has shown strong interest in a long-term partnership if the enterprise solution aligns with his company’s compliance and integration needs. He mentioned that decision-making will involve multiple stakeholders, and the procurement cycle might take up to three months. We should prepare detailed documentation, case studies, and a tailored presentation for his board of directors.</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
         </is>
       </c>
     </row>

</xml_diff>